<commit_message>
Authenticate/non-authenticate/FA/MD + logic + work
</commit_message>
<xml_diff>
--- a/Third Part - Physical Layer Device Authentication/Code/Simulations/1.xlsx
+++ b/Third Part - Physical Layer Device Authentication/Code/Simulations/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\ATCNS - vettore soglie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roves\OneDrive\Documenti\GitHub\ATCNS-Project\Third Part - Physical Layer Device Authentication\Code\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D91849-0F6F-4653-815C-77FF29E75100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80D2474-AA5E-4B47-975F-49291BD601FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E6EE1C6-235F-4E80-A1C2-C5C272370381}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E6EE1C6-235F-4E80-A1C2-C5C272370381}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Distanza (m)</t>
   </si>
@@ -70,12 +70,15 @@
   <si>
     <t>BER - Simulazione 10</t>
   </si>
+  <si>
+    <t>Media</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +86,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,11 +121,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -443,15 +462,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31050A5-C242-4255-8094-90056DD53635}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="22" max="22" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +507,11 @@
       <c r="T1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>0.44</v>
       </c>
@@ -518,8 +543,12 @@
       <c r="U2">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2" s="3">
+        <f>AVERAGE(B2:U2)</f>
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>0.39</v>
       </c>
@@ -551,8 +580,12 @@
       <c r="U3">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3" s="3">
+        <f t="shared" ref="V3:V31" si="0">AVERAGE(B3:U3)</f>
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>0.43</v>
       </c>
@@ -584,8 +617,12 @@
       <c r="U4">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>0.39</v>
       </c>
@@ -617,8 +654,12 @@
       <c r="U5">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48200000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>0.43</v>
       </c>
@@ -650,8 +691,12 @@
       <c r="U6">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49400000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>0.49</v>
       </c>
@@ -682,8 +727,12 @@
       <c r="U7">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49700000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>0.4</v>
       </c>
@@ -714,8 +763,12 @@
       <c r="U8">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>0.4</v>
       </c>
@@ -746,8 +799,12 @@
       <c r="U9">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4840000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>0.44</v>
       </c>
@@ -778,8 +835,12 @@
       <c r="U10">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48600000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>0.45</v>
       </c>
@@ -810,8 +871,12 @@
       <c r="U11">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49099999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>0.43</v>
       </c>
@@ -842,8 +907,12 @@
       <c r="U12">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>0.4</v>
       </c>
@@ -874,8 +943,12 @@
       <c r="U13">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47700000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>0.45</v>
       </c>
@@ -906,8 +979,12 @@
       <c r="U14">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48600000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>0.44</v>
       </c>
@@ -938,8 +1015,12 @@
       <c r="U15">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48600000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>0.37</v>
       </c>
@@ -970,8 +1051,12 @@
       <c r="U16">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48500000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>0.41</v>
       </c>
@@ -1002,8 +1087,12 @@
       <c r="U17">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>0.46</v>
       </c>
@@ -1034,8 +1123,12 @@
       <c r="U18">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47400000000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>0.47</v>
       </c>
@@ -1066,8 +1159,12 @@
       <c r="U19">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>0.39</v>
       </c>
@@ -1098,8 +1195,12 @@
       <c r="U20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>0.47</v>
       </c>
@@ -1130,8 +1231,12 @@
       <c r="U21">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>0.47</v>
       </c>
@@ -1162,8 +1267,12 @@
       <c r="U22">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V22" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4880000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>0.42</v>
       </c>
@@ -1194,8 +1303,12 @@
       <c r="U23">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V23" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>0.42</v>
       </c>
@@ -1226,8 +1339,12 @@
       <c r="U24">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V24" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48100000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>0.45</v>
       </c>
@@ -1258,8 +1375,12 @@
       <c r="U25">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V25" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4840000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>0.5</v>
       </c>
@@ -1290,8 +1411,12 @@
       <c r="U26">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V26" s="3">
+        <f t="shared" si="0"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>0.41</v>
       </c>
@@ -1322,8 +1447,12 @@
       <c r="U27">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V27" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48600000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>0.47</v>
       </c>
@@ -1354,8 +1483,12 @@
       <c r="U28">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V28" s="3">
+        <f t="shared" si="0"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>0.46</v>
       </c>
@@ -1386,8 +1519,12 @@
       <c r="U29">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48900000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>0.43</v>
       </c>
@@ -1418,8 +1555,12 @@
       <c r="U30">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="V30" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47800000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>0.41</v>
       </c>
@@ -1449,6 +1590,10 @@
       </c>
       <c r="U31">
         <v>0.45</v>
+      </c>
+      <c r="V31" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47600000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>